<commit_message>
final update for today
</commit_message>
<xml_diff>
--- a/Wilson Rides/Data Guide.xlsx
+++ b/Wilson Rides/Data Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmccall\Documents\GIT\Aging-and-Disability\Wilson Rides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D9F498-69BB-4EBC-BDE0-C57160316C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E6961E-99DA-44AF-A171-98479EA7D0DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0405D0AF-57D6-44C6-BB1C-249A29BD168C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0405D0AF-57D6-44C6-BB1C-249A29BD168C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="381">
   <si>
     <t>ID</t>
   </si>
@@ -1097,6 +1097,90 @@
   </si>
   <si>
     <t>geo_75+_movedabroad</t>
+  </si>
+  <si>
+    <t>Tenure Total Households Series</t>
+  </si>
+  <si>
+    <t>tenure_total_agehh_series</t>
+  </si>
+  <si>
+    <t>Tenure</t>
+  </si>
+  <si>
+    <t>B25007_001E</t>
+  </si>
+  <si>
+    <t>Tenure Total Owner Occupied</t>
+  </si>
+  <si>
+    <t>tenure_allowneroccupied</t>
+  </si>
+  <si>
+    <t>B25007_002E</t>
+  </si>
+  <si>
+    <t>Tenure Owner Occupied 65 to 74</t>
+  </si>
+  <si>
+    <t>tenure_owner_65to74</t>
+  </si>
+  <si>
+    <t>B25007_009E</t>
+  </si>
+  <si>
+    <t>Tenure Owner Occupied 75 to 84</t>
+  </si>
+  <si>
+    <t>tenure_owner_75to84</t>
+  </si>
+  <si>
+    <t>B25007_010E</t>
+  </si>
+  <si>
+    <t>Tenure Owner Occupied 85+</t>
+  </si>
+  <si>
+    <t>tenure_owner_85+</t>
+  </si>
+  <si>
+    <t>B25007_011E</t>
+  </si>
+  <si>
+    <t>Tenure Total Renter Occupied</t>
+  </si>
+  <si>
+    <t>tenure_allrenteroccupied</t>
+  </si>
+  <si>
+    <t>B25007_012E</t>
+  </si>
+  <si>
+    <t>Tenure Renter Occupied 65 to 74</t>
+  </si>
+  <si>
+    <t>tenure_renter_65to74</t>
+  </si>
+  <si>
+    <t>B25007_019E</t>
+  </si>
+  <si>
+    <t>Tenure Renter Occupied 75 to 84</t>
+  </si>
+  <si>
+    <t>tenure_renter_75to84</t>
+  </si>
+  <si>
+    <t>B25007_020E</t>
+  </si>
+  <si>
+    <t>Tenure Renter Occupied 85+</t>
+  </si>
+  <si>
+    <t>tenure_renter_85+</t>
+  </si>
+  <si>
+    <t>B25007_021E</t>
   </si>
 </sst>
 </file>
@@ -1463,10 +1547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E928985-CBB8-499D-B847-9B7B73480E5B}">
-  <dimension ref="A1:E114"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:C60"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115:C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3416,6 +3500,159 @@
         <v>316</v>
       </c>
     </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>353</v>
+      </c>
+      <c r="C115" t="s">
+        <v>354</v>
+      </c>
+      <c r="D115" t="s">
+        <v>355</v>
+      </c>
+      <c r="E115" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>357</v>
+      </c>
+      <c r="C116" t="s">
+        <v>358</v>
+      </c>
+      <c r="D116" t="s">
+        <v>355</v>
+      </c>
+      <c r="E116" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>360</v>
+      </c>
+      <c r="C117" t="s">
+        <v>361</v>
+      </c>
+      <c r="D117" t="s">
+        <v>355</v>
+      </c>
+      <c r="E117" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>363</v>
+      </c>
+      <c r="C118" t="s">
+        <v>364</v>
+      </c>
+      <c r="D118" t="s">
+        <v>355</v>
+      </c>
+      <c r="E118" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>366</v>
+      </c>
+      <c r="C119" t="s">
+        <v>367</v>
+      </c>
+      <c r="D119" t="s">
+        <v>355</v>
+      </c>
+      <c r="E119" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>369</v>
+      </c>
+      <c r="C120" t="s">
+        <v>370</v>
+      </c>
+      <c r="D120" t="s">
+        <v>355</v>
+      </c>
+      <c r="E120" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>372</v>
+      </c>
+      <c r="C121" t="s">
+        <v>373</v>
+      </c>
+      <c r="D121" t="s">
+        <v>355</v>
+      </c>
+      <c r="E121" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>375</v>
+      </c>
+      <c r="C122" t="s">
+        <v>376</v>
+      </c>
+      <c r="D122" t="s">
+        <v>355</v>
+      </c>
+      <c r="E122" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>378</v>
+      </c>
+      <c r="C123" t="s">
+        <v>379</v>
+      </c>
+      <c r="D123" t="s">
+        <v>355</v>
+      </c>
+      <c r="E123" t="s">
+        <v>380</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>